<commit_message>
Add test cases and common data providers
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -7,79 +7,16 @@
     <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
-    <sheet name="test_suite" sheetId="3" r:id="rId3"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId2"/>
+    <sheet name="CreateAccountTest" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Ivanov</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>postcode</t>
-  </si>
-  <si>
-    <t>alerttext</t>
-  </si>
-  <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Dollar</t>
-  </si>
-  <si>
-    <t>Ivan Ivanov</t>
-  </si>
-  <si>
-    <t>Account created successfully</t>
-  </si>
-  <si>
-    <t>Petya</t>
-  </si>
-  <si>
-    <t>Petrov</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>Sidor</t>
-  </si>
-  <si>
-    <t>Sidorov</t>
-  </si>
-  <si>
-    <t>sdsagg4</t>
-  </si>
-  <si>
-    <t>Kirill</t>
-  </si>
-  <si>
-    <t>Kirillov</t>
-  </si>
-  <si>
-    <t>sdfgre34</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>TCID</t>
   </si>
@@ -90,29 +27,38 @@
     <t>Y</t>
   </si>
   <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>runmode</t>
   </si>
   <si>
     <t>LoginTest</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>trainer@way2automation.com</t>
+  </si>
+  <si>
+    <t>Selenium@123</t>
+  </si>
+  <si>
+    <t>CreateAccountTest</t>
+  </si>
+  <si>
+    <t>accountname</t>
+  </si>
+  <si>
+    <t>Alex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +66,14 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,13 +93,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,154 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>123123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -595,42 +411,100 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>